<commit_message>
Fix the design so it generates a correct BOM
</commit_message>
<xml_diff>
--- a/Production/GATEWY.PCB.bom.xlsx
+++ b/Production/GATEWY.PCB.bom.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="GATEWY.PCB" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="GATEWY.PCB.bom" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="103">
   <si>
     <t>Part</t>
   </si>
@@ -139,7 +139,16 @@
     <t>JTAG</t>
   </si>
   <si>
-    <t>2X10JTAG</t>
+    <t>2X10JTAGSMD</t>
+  </si>
+  <si>
+    <t>2X10JTAG-SMD</t>
+  </si>
+  <si>
+    <t>Sullins</t>
+  </si>
+  <si>
+    <t>GRPB102VWQS-RC</t>
   </si>
   <si>
     <t>KW2</t>
@@ -178,6 +187,12 @@
     <t>RGBLED</t>
   </si>
   <si>
+    <t>Cree</t>
+  </si>
+  <si>
+    <t>CLV1A-FKB-CK1N1G1BB7R4S3</t>
+  </si>
+  <si>
     <t>R1</t>
   </si>
   <si>
@@ -253,16 +268,10 @@
     <t>RA_BUTTON</t>
   </si>
   <si>
-    <t>SWD</t>
-  </si>
-  <si>
-    <t>PINHD-2X5SMALL</t>
-  </si>
-  <si>
-    <t>2X5HDR</t>
-  </si>
-  <si>
-    <t>PIN HEADER</t>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>2-1825027-0</t>
   </si>
   <si>
     <t>U$14</t>
@@ -274,10 +283,7 @@
     <t>FIDUCIAL_1MM</t>
   </si>
   <si>
-    <t>For use by pick and place machines to calibrate the vision/machine</t>
-  </si>
-  <si>
-    <t> 1mm</t>
+    <t>For use by pick and place machines to calibrate the vision/machine, 1mm</t>
   </si>
   <si>
     <t>DNP</t>
@@ -305,6 +311,9 @@
   </si>
   <si>
     <t>SO14</t>
+  </si>
+  <si>
+    <t>WorldSemi</t>
   </si>
   <si>
     <t>X1</t>
@@ -415,7 +424,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:K32"/>
+  <dimension ref="A3:J31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -423,17 +432,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2397959183673"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="16.3163265306122"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6581632653061"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="64.3979591836735"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.2959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.0867346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.7551020408163"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.48469387755102"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.40816326530612"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.05612244897959"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="5.15816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -683,381 +691,373 @@
         <v>39</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>18</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="C18" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>80</v>
+        <v>87</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="K25" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="K26" s="0" t="s">
-        <v>86</v>
+      <c r="J26" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J27" s="0" t="s">
         <v>88</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="K27" s="0" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="K28" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="K29" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>95</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="K30" s="0" t="s">
-        <v>86</v>
+        <v>97</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>